<commit_message>
Add check CR and LFin scenario and temporal reference
</commit_message>
<xml_diff>
--- a/input_data/data_errors_2/3_cenarios_e_referencia_temporal/cenarios.xlsx
+++ b/input_data/data_errors_2/3_cenarios_e_referencia_temporal/cenarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>nome</t>
   </si>
@@ -28,7 +28,8 @@
     <t>Otimista</t>
   </si>
   <si>
-    <t>Este cenário representa uma visão mais otimista, sendo baseado em um menor crescimento populacional, menor desmatamento, menor consumo, etc.</t>
+    <t>Este cenário representa uma visão mais 
+otimista, sendo baseado em um menor crescimento populacional, menor desmatamento, menor consumo, etc.</t>
   </si>
   <si>
     <t>O</t>
@@ -37,10 +38,10 @@
     <t>Pessimista</t>
   </si>
   <si>
-    <t>Este cenário representa uma visão mais pessimista, sendo baseado em um maior crescimento populacional, maior desmatamento, maior consumo etc.</t>
+    <t>P</t>
   </si>
   <si>
-    <t>P</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -117,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -133,6 +134,9 @@
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,23 +457,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="24.649999999999995" customFormat="1" s="1">
@@ -527,10 +531,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -549,7 +553,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -567,7 +573,7 @@
       <c r="Q4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -586,7 +592,7 @@
       <c r="Q5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -605,7 +611,7 @@
       <c r="Q6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -623,8 +629,8 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="134.25">
-      <c r="A8" s="6"/>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -642,8 +648,8 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="95.25">
-      <c r="A9" s="6"/>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="7"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -662,7 +668,7 @@
       <c r="Q9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="72.75">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -681,7 +687,7 @@
       <c r="Q10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="75">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -700,7 +706,7 @@
       <c r="Q11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="67.5">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -719,7 +725,7 @@
       <c r="Q12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="59.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -738,7 +744,7 @@
       <c r="Q13" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="14.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -16755,42 +16761,42 @@
       <c r="Q856" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="857" customHeight="1" ht="16.5">
-      <c r="A857" s="7"/>
-      <c r="B857" s="7"/>
-      <c r="C857" s="7"/>
-      <c r="D857" s="7"/>
-      <c r="E857" s="7"/>
-      <c r="F857" s="7"/>
-      <c r="G857" s="7"/>
-      <c r="H857" s="7"/>
-      <c r="I857" s="7"/>
-      <c r="J857" s="7"/>
-      <c r="K857" s="7"/>
-      <c r="L857" s="7"/>
-      <c r="M857" s="7"/>
-      <c r="N857" s="7"/>
-      <c r="O857" s="7"/>
-      <c r="P857" s="7"/>
-      <c r="Q857" s="7"/>
+      <c r="A857" s="8"/>
+      <c r="B857" s="8"/>
+      <c r="C857" s="8"/>
+      <c r="D857" s="8"/>
+      <c r="E857" s="8"/>
+      <c r="F857" s="8"/>
+      <c r="G857" s="8"/>
+      <c r="H857" s="8"/>
+      <c r="I857" s="8"/>
+      <c r="J857" s="8"/>
+      <c r="K857" s="8"/>
+      <c r="L857" s="8"/>
+      <c r="M857" s="8"/>
+      <c r="N857" s="8"/>
+      <c r="O857" s="8"/>
+      <c r="P857" s="8"/>
+      <c r="Q857" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="858" customHeight="1" ht="15.75">
-      <c r="A858" s="7"/>
-      <c r="B858" s="7"/>
-      <c r="C858" s="7"/>
-      <c r="D858" s="7"/>
-      <c r="E858" s="7"/>
-      <c r="F858" s="7"/>
-      <c r="G858" s="7"/>
-      <c r="H858" s="7"/>
-      <c r="I858" s="7"/>
-      <c r="J858" s="7"/>
-      <c r="K858" s="7"/>
-      <c r="L858" s="7"/>
-      <c r="M858" s="7"/>
-      <c r="N858" s="7"/>
-      <c r="O858" s="7"/>
-      <c r="P858" s="7"/>
-      <c r="Q858" s="7"/>
+      <c r="A858" s="8"/>
+      <c r="B858" s="8"/>
+      <c r="C858" s="8"/>
+      <c r="D858" s="8"/>
+      <c r="E858" s="8"/>
+      <c r="F858" s="8"/>
+      <c r="G858" s="8"/>
+      <c r="H858" s="8"/>
+      <c r="I858" s="8"/>
+      <c r="J858" s="8"/>
+      <c r="K858" s="8"/>
+      <c r="L858" s="8"/>
+      <c r="M858" s="8"/>
+      <c r="N858" s="8"/>
+      <c r="O858" s="8"/>
+      <c r="P858" s="8"/>
+      <c r="Q858" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>